<commit_message>
Manje promene: powerPoint, CV u pdf-u, promena imena u budzetu
</commit_message>
<xml_diff>
--- a/2b Format partner budget - Horizon2020.xlsx
+++ b/2b Format partner budget - Horizon2020.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ana\Downloads\Projekat_Faza1_ver1 (2)\Projekat_Faza1_ver1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ana\Desktop\USP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D90FF4-D93E-4E04-B574-B58DADE81E7F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17F5F66-ED5C-419E-A83E-04C2CF5206B3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" tabRatio="525" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="525" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Detaljno budzet-ETF" sheetId="1" r:id="rId1"/>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="141">
   <si>
     <t>Partner budget Horizon 2020</t>
   </si>
@@ -520,6 +520,12 @@
   </si>
   <si>
     <t>114953</t>
+  </si>
+  <si>
+    <t>DeSmartEm</t>
+  </si>
+  <si>
+    <t>Oprema za kancelarije, održavanje prostorija...</t>
   </si>
 </sst>
 </file>
@@ -637,7 +643,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1023,9 +1028,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1046,60 +1098,13 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
@@ -1630,8 +1635,8 @@
   </sheetPr>
   <dimension ref="A1:T40"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34:P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1656,69 +1661,71 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D4" s="2"/>
-      <c r="E4" s="63" t="s">
+      <c r="E4" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="51"/>
-      <c r="L4" s="64" t="s">
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="51" t="s">
+        <v>139</v>
+      </c>
+      <c r="L4" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="64"/>
-      <c r="N4" s="64"/>
+      <c r="M4" s="79"/>
+      <c r="N4" s="79"/>
       <c r="O4" s="4">
         <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D5" s="2"/>
-      <c r="E5" s="63" t="s">
+      <c r="E5" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="64"/>
-      <c r="G5" s="64"/>
-      <c r="H5" s="64"/>
-      <c r="I5" s="64"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="79"/>
       <c r="J5" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="L5" s="64" t="s">
+      <c r="L5" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="M5" s="64"/>
-      <c r="N5" s="64"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="79"/>
       <c r="O5" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D6" s="2"/>
-      <c r="E6" s="63" t="s">
+      <c r="E6" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="64"/>
-      <c r="I6" s="64"/>
+      <c r="F6" s="79"/>
+      <c r="G6" s="79"/>
+      <c r="H6" s="79"/>
+      <c r="I6" s="79"/>
       <c r="J6" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="L6" s="64" t="s">
+      <c r="L6" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="M6" s="64"/>
-      <c r="N6" s="64"/>
+      <c r="M6" s="79"/>
+      <c r="N6" s="79"/>
       <c r="O6" s="5">
         <v>1</v>
       </c>
@@ -1728,21 +1735,21 @@
       <c r="Q6" s="6"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="E7" s="64" t="s">
+      <c r="E7" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="64"/>
-      <c r="G7" s="64"/>
-      <c r="H7" s="64"/>
-      <c r="I7" s="64"/>
+      <c r="F7" s="79"/>
+      <c r="G7" s="79"/>
+      <c r="H7" s="79"/>
+      <c r="I7" s="79"/>
       <c r="J7" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="L7" s="64" t="s">
+      <c r="L7" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="64"/>
-      <c r="N7" s="64"/>
+      <c r="M7" s="79"/>
+      <c r="N7" s="79"/>
       <c r="O7" s="4">
         <v>1</v>
       </c>
@@ -1753,26 +1760,26 @@
     </row>
     <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="10" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="65" t="s">
+      <c r="A10" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="66"/>
-      <c r="C10" s="66"/>
-      <c r="D10" s="66"/>
-      <c r="E10" s="66"/>
-      <c r="F10" s="66"/>
-      <c r="G10" s="66"/>
-      <c r="H10" s="66"/>
-      <c r="I10" s="66"/>
-      <c r="J10" s="66"/>
-      <c r="K10" s="66"/>
-      <c r="L10" s="66"/>
-      <c r="M10" s="66"/>
-      <c r="N10" s="66"/>
-      <c r="O10" s="66"/>
-      <c r="P10" s="66"/>
-      <c r="Q10" s="66"/>
-      <c r="R10" s="66"/>
+      <c r="B10" s="81"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="81"/>
+      <c r="E10" s="81"/>
+      <c r="F10" s="81"/>
+      <c r="G10" s="81"/>
+      <c r="H10" s="81"/>
+      <c r="I10" s="81"/>
+      <c r="J10" s="81"/>
+      <c r="K10" s="81"/>
+      <c r="L10" s="81"/>
+      <c r="M10" s="81"/>
+      <c r="N10" s="81"/>
+      <c r="O10" s="81"/>
+      <c r="P10" s="81"/>
+      <c r="Q10" s="81"/>
+      <c r="R10" s="81"/>
       <c r="S10" s="8"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
@@ -1784,33 +1791,33 @@
       </c>
     </row>
     <row r="12" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D12" s="67" t="s">
+      <c r="D12" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="67"/>
-      <c r="F12" s="67"/>
-      <c r="G12" s="67"/>
-      <c r="H12" s="67"/>
-      <c r="I12" s="67"/>
-      <c r="J12" s="68" t="s">
+      <c r="E12" s="82"/>
+      <c r="F12" s="82"/>
+      <c r="G12" s="82"/>
+      <c r="H12" s="82"/>
+      <c r="I12" s="82"/>
+      <c r="J12" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="68"/>
-      <c r="L12" s="68"/>
-      <c r="M12" s="68"/>
-      <c r="N12" s="68"/>
-      <c r="O12" s="68"/>
-      <c r="P12" s="68"/>
-      <c r="Q12" s="68"/>
-      <c r="R12" s="68"/>
+      <c r="K12" s="83"/>
+      <c r="L12" s="83"/>
+      <c r="M12" s="83"/>
+      <c r="N12" s="83"/>
+      <c r="O12" s="83"/>
+      <c r="P12" s="83"/>
+      <c r="Q12" s="83"/>
+      <c r="R12" s="83"/>
       <c r="S12" s="9"/>
     </row>
     <row r="13" spans="1:19" s="14" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="61" t="s">
+      <c r="A13" s="76" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="61"/>
-      <c r="C13" s="61"/>
+      <c r="B13" s="76"/>
+      <c r="C13" s="76"/>
       <c r="D13" s="53" t="s">
         <v>62</v>
       </c>
@@ -1861,11 +1868,11 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" s="70" t="s">
+      <c r="A14" s="71" t="s">
         <v>85</v>
       </c>
-      <c r="B14" s="70"/>
-      <c r="C14" s="70"/>
+      <c r="B14" s="71"/>
+      <c r="C14" s="71"/>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
@@ -1881,7 +1888,7 @@
         <f>27*1750</f>
         <v>47250</v>
       </c>
-      <c r="K14" s="60">
+      <c r="K14" s="59">
         <f>20658*1+8000</f>
         <v>28658</v>
       </c>
@@ -1912,11 +1919,11 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" s="70" t="s">
+      <c r="A15" s="71" t="s">
         <v>130</v>
       </c>
-      <c r="B15" s="70"/>
-      <c r="C15" s="70"/>
+      <c r="B15" s="71"/>
+      <c r="C15" s="71"/>
       <c r="D15" s="15">
         <v>1</v>
       </c>
@@ -1966,11 +1973,11 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16" s="70" t="s">
+      <c r="A16" s="71" t="s">
         <v>86</v>
       </c>
-      <c r="B16" s="70"/>
-      <c r="C16" s="70"/>
+      <c r="B16" s="71"/>
+      <c r="C16" s="71"/>
       <c r="D16" s="15">
         <v>2</v>
       </c>
@@ -2018,11 +2025,11 @@
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A17" s="70" t="s">
+      <c r="A17" s="71" t="s">
         <v>87</v>
       </c>
-      <c r="B17" s="70"/>
-      <c r="C17" s="70"/>
+      <c r="B17" s="71"/>
+      <c r="C17" s="71"/>
       <c r="D17" s="15">
         <v>3</v>
       </c>
@@ -2072,11 +2079,11 @@
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A18" s="70" t="s">
+      <c r="A18" s="71" t="s">
         <v>88</v>
       </c>
-      <c r="B18" s="70"/>
-      <c r="C18" s="70"/>
+      <c r="B18" s="71"/>
+      <c r="C18" s="71"/>
       <c r="D18" s="15">
         <v>1</v>
       </c>
@@ -2120,11 +2127,11 @@
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A19" s="70" t="s">
+      <c r="A19" s="71" t="s">
         <v>89</v>
       </c>
-      <c r="B19" s="70"/>
-      <c r="C19" s="70"/>
+      <c r="B19" s="71"/>
+      <c r="C19" s="71"/>
       <c r="D19" s="15">
         <v>7</v>
       </c>
@@ -2172,11 +2179,11 @@
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A20" s="70" t="s">
+      <c r="A20" s="71" t="s">
         <v>90</v>
       </c>
-      <c r="B20" s="70"/>
-      <c r="C20" s="70"/>
+      <c r="B20" s="71"/>
+      <c r="C20" s="71"/>
       <c r="D20" s="15">
         <v>3</v>
       </c>
@@ -2222,11 +2229,11 @@
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A21" s="70" t="s">
+      <c r="A21" s="71" t="s">
         <v>91</v>
       </c>
-      <c r="B21" s="70"/>
-      <c r="C21" s="70"/>
+      <c r="B21" s="71"/>
+      <c r="C21" s="71"/>
       <c r="D21" s="15"/>
       <c r="E21" s="15">
         <v>6</v>
@@ -2268,11 +2275,11 @@
       </c>
     </row>
     <row r="22" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="70" t="s">
+      <c r="A22" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="70"/>
-      <c r="C22" s="70"/>
+      <c r="B22" s="71"/>
+      <c r="C22" s="71"/>
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
@@ -2303,11 +2310,11 @@
       </c>
     </row>
     <row r="23" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="70" t="s">
+      <c r="A23" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="70"/>
-      <c r="C23" s="70"/>
+      <c r="B23" s="71"/>
+      <c r="C23" s="71"/>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
@@ -2338,11 +2345,11 @@
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A24" s="71" t="s">
+      <c r="A24" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="71"/>
-      <c r="C24" s="71"/>
+      <c r="B24" s="75"/>
+      <c r="C24" s="75"/>
       <c r="D24" s="15">
         <f>SUM(D14:D23)</f>
         <v>17</v>
@@ -2463,24 +2470,24 @@
       <c r="S27" s="31"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A28" s="69" t="s">
+      <c r="A28" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="69"/>
-      <c r="C28" s="69"/>
-      <c r="D28" s="69"/>
-      <c r="E28" s="69"/>
-      <c r="F28" s="69"/>
-      <c r="G28" s="69"/>
-      <c r="H28" s="69"/>
-      <c r="I28" s="69"/>
-      <c r="J28" s="69"/>
-      <c r="K28" s="69"/>
-      <c r="L28" s="69"/>
-      <c r="M28" s="69"/>
-      <c r="N28" s="69"/>
-      <c r="O28" s="69"/>
-      <c r="P28" s="69"/>
+      <c r="B28" s="74"/>
+      <c r="C28" s="74"/>
+      <c r="D28" s="74"/>
+      <c r="E28" s="74"/>
+      <c r="F28" s="74"/>
+      <c r="G28" s="74"/>
+      <c r="H28" s="74"/>
+      <c r="I28" s="74"/>
+      <c r="J28" s="74"/>
+      <c r="K28" s="74"/>
+      <c r="L28" s="74"/>
+      <c r="M28" s="74"/>
+      <c r="N28" s="74"/>
+      <c r="O28" s="74"/>
+      <c r="P28" s="74"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="32"/>
@@ -2521,101 +2528,103 @@
       <c r="P30" s="32"/>
     </row>
     <row r="31" spans="1:20" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="72" t="str">
+      <c r="A31" s="67" t="str">
         <f>CONCATENATE("participant"," ",J6)</f>
         <v>participant ETF</v>
       </c>
-      <c r="B31" s="73"/>
+      <c r="B31" s="68"/>
       <c r="C31" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D31" s="70" t="s">
+      <c r="D31" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="E31" s="74"/>
-      <c r="F31" s="74"/>
-      <c r="G31" s="74"/>
-      <c r="H31" s="74"/>
-      <c r="I31" s="74"/>
-      <c r="J31" s="74"/>
-      <c r="K31" s="74"/>
-      <c r="L31" s="74"/>
-      <c r="M31" s="74"/>
-      <c r="N31" s="74"/>
-      <c r="O31" s="74"/>
-      <c r="P31" s="74"/>
+      <c r="E31" s="72"/>
+      <c r="F31" s="72"/>
+      <c r="G31" s="72"/>
+      <c r="H31" s="72"/>
+      <c r="I31" s="72"/>
+      <c r="J31" s="72"/>
+      <c r="K31" s="72"/>
+      <c r="L31" s="72"/>
+      <c r="M31" s="72"/>
+      <c r="N31" s="72"/>
+      <c r="O31" s="72"/>
+      <c r="P31" s="72"/>
     </row>
     <row r="32" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="75" t="s">
+      <c r="A32" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="75"/>
+      <c r="B32" s="61"/>
       <c r="C32" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="D32" s="76" t="s">
+      <c r="D32" s="73" t="s">
         <v>59</v>
       </c>
-      <c r="E32" s="77"/>
-      <c r="F32" s="77"/>
-      <c r="G32" s="77"/>
-      <c r="H32" s="77"/>
-      <c r="I32" s="77"/>
-      <c r="J32" s="77"/>
-      <c r="K32" s="77"/>
-      <c r="L32" s="77"/>
-      <c r="M32" s="77"/>
-      <c r="N32" s="77"/>
-      <c r="O32" s="77"/>
-      <c r="P32" s="77"/>
+      <c r="E32" s="66"/>
+      <c r="F32" s="66"/>
+      <c r="G32" s="66"/>
+      <c r="H32" s="66"/>
+      <c r="I32" s="66"/>
+      <c r="J32" s="66"/>
+      <c r="K32" s="66"/>
+      <c r="L32" s="66"/>
+      <c r="M32" s="66"/>
+      <c r="N32" s="66"/>
+      <c r="O32" s="66"/>
+      <c r="P32" s="66"/>
       <c r="S32" s="31"/>
     </row>
     <row r="33" spans="1:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="75" t="s">
+      <c r="A33" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="75"/>
+      <c r="B33" s="61"/>
       <c r="C33" s="35">
         <v>67000</v>
       </c>
-      <c r="D33" s="77" t="s">
+      <c r="D33" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="E33" s="77"/>
-      <c r="F33" s="77"/>
-      <c r="G33" s="77"/>
-      <c r="H33" s="77"/>
-      <c r="I33" s="77"/>
-      <c r="J33" s="77"/>
-      <c r="K33" s="77"/>
-      <c r="L33" s="77"/>
-      <c r="M33" s="77"/>
-      <c r="N33" s="77"/>
-      <c r="O33" s="77"/>
-      <c r="P33" s="77"/>
+      <c r="E33" s="66"/>
+      <c r="F33" s="66"/>
+      <c r="G33" s="66"/>
+      <c r="H33" s="66"/>
+      <c r="I33" s="66"/>
+      <c r="J33" s="66"/>
+      <c r="K33" s="66"/>
+      <c r="L33" s="66"/>
+      <c r="M33" s="66"/>
+      <c r="N33" s="66"/>
+      <c r="O33" s="66"/>
+      <c r="P33" s="66"/>
       <c r="S33" s="31"/>
     </row>
     <row r="34" spans="1:19" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="75" t="s">
+      <c r="A34" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="75"/>
+      <c r="B34" s="61"/>
       <c r="C34" s="35">
         <v>8000</v>
       </c>
-      <c r="D34" s="77"/>
-      <c r="E34" s="77"/>
-      <c r="F34" s="77"/>
-      <c r="G34" s="77"/>
-      <c r="H34" s="77"/>
-      <c r="I34" s="77"/>
-      <c r="J34" s="77"/>
-      <c r="K34" s="77"/>
-      <c r="L34" s="77"/>
-      <c r="M34" s="77"/>
-      <c r="N34" s="77"/>
-      <c r="O34" s="77"/>
-      <c r="P34" s="77"/>
+      <c r="D34" s="66" t="s">
+        <v>140</v>
+      </c>
+      <c r="E34" s="66"/>
+      <c r="F34" s="66"/>
+      <c r="G34" s="66"/>
+      <c r="H34" s="66"/>
+      <c r="I34" s="66"/>
+      <c r="J34" s="66"/>
+      <c r="K34" s="66"/>
+      <c r="L34" s="66"/>
+      <c r="M34" s="66"/>
+      <c r="N34" s="66"/>
+      <c r="O34" s="66"/>
+      <c r="P34" s="66"/>
       <c r="S34" s="31"/>
     </row>
     <row r="35" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
@@ -2649,134 +2658,106 @@
       <c r="P36" s="38"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A37" s="72" t="str">
+      <c r="A37" s="67" t="str">
         <f>CONCATENATE("participant"," ",C9)</f>
         <v xml:space="preserve">participant </v>
       </c>
-      <c r="B37" s="73"/>
+      <c r="B37" s="68"/>
       <c r="C37" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D37" s="82" t="s">
+      <c r="D37" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="E37" s="83"/>
-      <c r="F37" s="83"/>
-      <c r="G37" s="83"/>
-      <c r="H37" s="83"/>
-      <c r="I37" s="83"/>
-      <c r="J37" s="83"/>
-      <c r="K37" s="83"/>
-      <c r="L37" s="83"/>
-      <c r="M37" s="83"/>
-      <c r="N37" s="83"/>
-      <c r="O37" s="83"/>
-      <c r="P37" s="83"/>
+      <c r="E37" s="70"/>
+      <c r="F37" s="70"/>
+      <c r="G37" s="70"/>
+      <c r="H37" s="70"/>
+      <c r="I37" s="70"/>
+      <c r="J37" s="70"/>
+      <c r="K37" s="70"/>
+      <c r="L37" s="70"/>
+      <c r="M37" s="70"/>
+      <c r="N37" s="70"/>
+      <c r="O37" s="70"/>
+      <c r="P37" s="70"/>
     </row>
     <row r="38" spans="1:19" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="75" t="s">
+      <c r="A38" s="61" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="75"/>
+      <c r="B38" s="61"/>
       <c r="C38" s="35">
         <v>40000</v>
       </c>
-      <c r="D38" s="81" t="s">
+      <c r="D38" s="65" t="s">
         <v>61</v>
       </c>
-      <c r="E38" s="77"/>
-      <c r="F38" s="77"/>
-      <c r="G38" s="77"/>
-      <c r="H38" s="77"/>
-      <c r="I38" s="77"/>
-      <c r="J38" s="77"/>
-      <c r="K38" s="77"/>
-      <c r="L38" s="77"/>
-      <c r="M38" s="77"/>
-      <c r="N38" s="77"/>
-      <c r="O38" s="77"/>
-      <c r="P38" s="77"/>
+      <c r="E38" s="66"/>
+      <c r="F38" s="66"/>
+      <c r="G38" s="66"/>
+      <c r="H38" s="66"/>
+      <c r="I38" s="66"/>
+      <c r="J38" s="66"/>
+      <c r="K38" s="66"/>
+      <c r="L38" s="66"/>
+      <c r="M38" s="66"/>
+      <c r="N38" s="66"/>
+      <c r="O38" s="66"/>
+      <c r="P38" s="66"/>
       <c r="S38" s="31"/>
     </row>
     <row r="39" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="75" t="s">
+      <c r="A39" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="75"/>
+      <c r="B39" s="61"/>
       <c r="C39" s="35"/>
-      <c r="D39" s="78" t="s">
+      <c r="D39" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="E39" s="79"/>
-      <c r="F39" s="79"/>
-      <c r="G39" s="79"/>
-      <c r="H39" s="79"/>
-      <c r="I39" s="79"/>
-      <c r="J39" s="79"/>
-      <c r="K39" s="79"/>
-      <c r="L39" s="79"/>
-      <c r="M39" s="79"/>
-      <c r="N39" s="79"/>
-      <c r="O39" s="79"/>
-      <c r="P39" s="80"/>
+      <c r="E39" s="63"/>
+      <c r="F39" s="63"/>
+      <c r="G39" s="63"/>
+      <c r="H39" s="63"/>
+      <c r="I39" s="63"/>
+      <c r="J39" s="63"/>
+      <c r="K39" s="63"/>
+      <c r="L39" s="63"/>
+      <c r="M39" s="63"/>
+      <c r="N39" s="63"/>
+      <c r="O39" s="63"/>
+      <c r="P39" s="64"/>
       <c r="S39" s="31"/>
     </row>
     <row r="40" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="75" t="s">
+      <c r="A40" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="75"/>
+      <c r="B40" s="61"/>
       <c r="C40" s="35"/>
-      <c r="D40" s="81" t="s">
+      <c r="D40" s="65" t="s">
         <v>41</v>
       </c>
-      <c r="E40" s="77"/>
-      <c r="F40" s="77"/>
-      <c r="G40" s="77"/>
-      <c r="H40" s="77"/>
-      <c r="I40" s="77"/>
-      <c r="J40" s="77"/>
-      <c r="K40" s="77"/>
-      <c r="L40" s="77"/>
-      <c r="M40" s="77"/>
-      <c r="N40" s="77"/>
-      <c r="O40" s="77"/>
-      <c r="P40" s="77"/>
+      <c r="E40" s="66"/>
+      <c r="F40" s="66"/>
+      <c r="G40" s="66"/>
+      <c r="H40" s="66"/>
+      <c r="I40" s="66"/>
+      <c r="J40" s="66"/>
+      <c r="K40" s="66"/>
+      <c r="L40" s="66"/>
+      <c r="M40" s="66"/>
+      <c r="N40" s="66"/>
+      <c r="O40" s="66"/>
+      <c r="P40" s="66"/>
       <c r="S40" s="31"/>
     </row>
   </sheetData>
   <protectedRanges>
-    <protectedRange sqref="C32:P40 D14:H23 P14:P23 O6 J14:N23 R14:S23" name="Range1"/>
+    <protectedRange sqref="C32:P40 D14:H23 P14:P23 O6 R14:S23 J14:N23" name="Range1"/>
   </protectedRanges>
   <mergeCells count="41">
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:P39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:P40"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D34:P34"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:P37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:P38"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:P31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:P32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:P33"/>
-    <mergeCell ref="A28:P28"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:C24"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="E3:I3"/>
     <mergeCell ref="E4:I4"/>
@@ -2790,6 +2771,34 @@
     <mergeCell ref="A10:R10"/>
     <mergeCell ref="D12:I12"/>
     <mergeCell ref="J12:R12"/>
+    <mergeCell ref="A28:P28"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:P31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:P32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:P33"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:P39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:P40"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D34:P34"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:P37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:P38"/>
   </mergeCells>
   <conditionalFormatting sqref="O4">
     <cfRule type="expression" dxfId="1" priority="1">
@@ -2815,8 +2824,8 @@
   </sheetPr>
   <dimension ref="A1:T40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2839,69 +2848,71 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D4" s="2"/>
-      <c r="E4" s="63" t="s">
+      <c r="E4" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="51"/>
-      <c r="L4" s="64" t="s">
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="51" t="s">
+        <v>139</v>
+      </c>
+      <c r="L4" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="64"/>
-      <c r="N4" s="64"/>
+      <c r="M4" s="79"/>
+      <c r="N4" s="79"/>
       <c r="O4" s="4">
         <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D5" s="2"/>
-      <c r="E5" s="63" t="s">
+      <c r="E5" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="64"/>
-      <c r="G5" s="64"/>
-      <c r="H5" s="64"/>
-      <c r="I5" s="64"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="79"/>
       <c r="J5" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="L5" s="64" t="s">
+      <c r="L5" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="M5" s="64"/>
-      <c r="N5" s="64"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="79"/>
       <c r="O5" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D6" s="2"/>
-      <c r="E6" s="63" t="s">
+      <c r="E6" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="64"/>
-      <c r="I6" s="64"/>
+      <c r="F6" s="79"/>
+      <c r="G6" s="79"/>
+      <c r="H6" s="79"/>
+      <c r="I6" s="79"/>
       <c r="J6" s="51" t="s">
         <v>94</v>
       </c>
-      <c r="L6" s="64" t="s">
+      <c r="L6" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="M6" s="64"/>
-      <c r="N6" s="64"/>
+      <c r="M6" s="79"/>
+      <c r="N6" s="79"/>
       <c r="O6" s="5">
         <v>0.7</v>
       </c>
@@ -2911,21 +2922,21 @@
       <c r="Q6" s="6"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="E7" s="64" t="s">
+      <c r="E7" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="64"/>
-      <c r="G7" s="64"/>
-      <c r="H7" s="64"/>
-      <c r="I7" s="64"/>
+      <c r="F7" s="79"/>
+      <c r="G7" s="79"/>
+      <c r="H7" s="79"/>
+      <c r="I7" s="79"/>
       <c r="J7" s="51" t="s">
         <v>135</v>
       </c>
-      <c r="L7" s="64" t="s">
+      <c r="L7" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="64"/>
-      <c r="N7" s="64"/>
+      <c r="M7" s="79"/>
+      <c r="N7" s="79"/>
       <c r="O7" s="4">
         <v>1</v>
       </c>
@@ -2936,56 +2947,56 @@
     </row>
     <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="10" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="65" t="s">
+      <c r="A10" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="66"/>
-      <c r="C10" s="66"/>
-      <c r="D10" s="66"/>
-      <c r="E10" s="66"/>
-      <c r="F10" s="66"/>
-      <c r="G10" s="66"/>
-      <c r="H10" s="66"/>
-      <c r="I10" s="66"/>
-      <c r="J10" s="66"/>
-      <c r="K10" s="66"/>
-      <c r="L10" s="66"/>
-      <c r="M10" s="66"/>
-      <c r="N10" s="66"/>
-      <c r="O10" s="66"/>
-      <c r="P10" s="66"/>
-      <c r="Q10" s="66"/>
-      <c r="R10" s="66"/>
+      <c r="B10" s="81"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="81"/>
+      <c r="E10" s="81"/>
+      <c r="F10" s="81"/>
+      <c r="G10" s="81"/>
+      <c r="H10" s="81"/>
+      <c r="I10" s="81"/>
+      <c r="J10" s="81"/>
+      <c r="K10" s="81"/>
+      <c r="L10" s="81"/>
+      <c r="M10" s="81"/>
+      <c r="N10" s="81"/>
+      <c r="O10" s="81"/>
+      <c r="P10" s="81"/>
+      <c r="Q10" s="81"/>
+      <c r="R10" s="81"/>
       <c r="S10" s="8"/>
     </row>
     <row r="12" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D12" s="67" t="s">
+      <c r="D12" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="67"/>
-      <c r="F12" s="67"/>
-      <c r="G12" s="67"/>
-      <c r="H12" s="67"/>
-      <c r="I12" s="67"/>
-      <c r="J12" s="68" t="s">
+      <c r="E12" s="82"/>
+      <c r="F12" s="82"/>
+      <c r="G12" s="82"/>
+      <c r="H12" s="82"/>
+      <c r="I12" s="82"/>
+      <c r="J12" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="68"/>
-      <c r="L12" s="68"/>
-      <c r="M12" s="68"/>
-      <c r="N12" s="68"/>
-      <c r="O12" s="68"/>
-      <c r="P12" s="68"/>
-      <c r="Q12" s="68"/>
-      <c r="R12" s="68"/>
+      <c r="K12" s="83"/>
+      <c r="L12" s="83"/>
+      <c r="M12" s="83"/>
+      <c r="N12" s="83"/>
+      <c r="O12" s="83"/>
+      <c r="P12" s="83"/>
+      <c r="Q12" s="83"/>
+      <c r="R12" s="83"/>
       <c r="S12" s="9"/>
     </row>
     <row r="13" spans="1:19" s="14" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="61" t="s">
+      <c r="A13" s="76" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="61"/>
-      <c r="C13" s="61"/>
+      <c r="B13" s="76"/>
+      <c r="C13" s="76"/>
       <c r="D13" s="53" t="s">
         <v>62</v>
       </c>
@@ -3036,11 +3047,11 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" s="70" t="s">
+      <c r="A14" s="71" t="s">
         <v>85</v>
       </c>
-      <c r="B14" s="70"/>
-      <c r="C14" s="70"/>
+      <c r="B14" s="71"/>
+      <c r="C14" s="71"/>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
@@ -3084,11 +3095,11 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" s="70" t="s">
+      <c r="A15" s="71" t="s">
         <v>130</v>
       </c>
-      <c r="B15" s="70"/>
-      <c r="C15" s="70"/>
+      <c r="B15" s="71"/>
+      <c r="C15" s="71"/>
       <c r="D15" s="15">
         <v>1</v>
       </c>
@@ -3134,11 +3145,11 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16" s="70" t="s">
+      <c r="A16" s="71" t="s">
         <v>86</v>
       </c>
-      <c r="B16" s="70"/>
-      <c r="C16" s="70"/>
+      <c r="B16" s="71"/>
+      <c r="C16" s="71"/>
       <c r="D16" s="15">
         <v>11</v>
       </c>
@@ -3184,11 +3195,11 @@
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A17" s="70" t="s">
+      <c r="A17" s="71" t="s">
         <v>87</v>
       </c>
-      <c r="B17" s="70"/>
-      <c r="C17" s="70"/>
+      <c r="B17" s="71"/>
+      <c r="C17" s="71"/>
       <c r="D17" s="15">
         <v>2</v>
       </c>
@@ -3234,11 +3245,11 @@
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A18" s="70" t="s">
+      <c r="A18" s="71" t="s">
         <v>88</v>
       </c>
-      <c r="B18" s="70"/>
-      <c r="C18" s="70"/>
+      <c r="B18" s="71"/>
+      <c r="C18" s="71"/>
       <c r="D18" s="15">
         <v>2</v>
       </c>
@@ -3282,11 +3293,11 @@
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A19" s="70" t="s">
+      <c r="A19" s="71" t="s">
         <v>89</v>
       </c>
-      <c r="B19" s="70"/>
-      <c r="C19" s="70"/>
+      <c r="B19" s="71"/>
+      <c r="C19" s="71"/>
       <c r="D19" s="15">
         <v>5</v>
       </c>
@@ -3333,11 +3344,11 @@
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A20" s="70" t="s">
+      <c r="A20" s="71" t="s">
         <v>90</v>
       </c>
-      <c r="B20" s="70"/>
-      <c r="C20" s="70"/>
+      <c r="B20" s="71"/>
+      <c r="C20" s="71"/>
       <c r="D20" s="15"/>
       <c r="E20" s="15">
         <v>2</v>
@@ -3379,11 +3390,11 @@
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A21" s="70" t="s">
+      <c r="A21" s="71" t="s">
         <v>91</v>
       </c>
-      <c r="B21" s="70"/>
-      <c r="C21" s="70"/>
+      <c r="B21" s="71"/>
+      <c r="C21" s="71"/>
       <c r="D21" s="15"/>
       <c r="E21" s="15">
         <v>2</v>
@@ -3427,11 +3438,11 @@
       </c>
     </row>
     <row r="22" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="70" t="s">
+      <c r="A22" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="70"/>
-      <c r="C22" s="70"/>
+      <c r="B22" s="71"/>
+      <c r="C22" s="71"/>
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
@@ -3462,11 +3473,11 @@
       </c>
     </row>
     <row r="23" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="70" t="s">
+      <c r="A23" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="70"/>
-      <c r="C23" s="70"/>
+      <c r="B23" s="71"/>
+      <c r="C23" s="71"/>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
@@ -3497,11 +3508,11 @@
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A24" s="71" t="s">
+      <c r="A24" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="71"/>
-      <c r="C24" s="71"/>
+      <c r="B24" s="75"/>
+      <c r="C24" s="75"/>
       <c r="D24" s="15">
         <f>SUM(D14:D23)</f>
         <v>21</v>
@@ -3622,24 +3633,24 @@
       <c r="S27" s="31"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A28" s="69" t="s">
+      <c r="A28" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="69"/>
-      <c r="C28" s="69"/>
-      <c r="D28" s="69"/>
-      <c r="E28" s="69"/>
-      <c r="F28" s="69"/>
-      <c r="G28" s="69"/>
-      <c r="H28" s="69"/>
-      <c r="I28" s="69"/>
-      <c r="J28" s="69"/>
-      <c r="K28" s="69"/>
-      <c r="L28" s="69"/>
-      <c r="M28" s="69"/>
-      <c r="N28" s="69"/>
-      <c r="O28" s="69"/>
-      <c r="P28" s="69"/>
+      <c r="B28" s="74"/>
+      <c r="C28" s="74"/>
+      <c r="D28" s="74"/>
+      <c r="E28" s="74"/>
+      <c r="F28" s="74"/>
+      <c r="G28" s="74"/>
+      <c r="H28" s="74"/>
+      <c r="I28" s="74"/>
+      <c r="J28" s="74"/>
+      <c r="K28" s="74"/>
+      <c r="L28" s="74"/>
+      <c r="M28" s="74"/>
+      <c r="N28" s="74"/>
+      <c r="O28" s="74"/>
+      <c r="P28" s="74"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="50"/>
@@ -3680,101 +3691,101 @@
       <c r="P30" s="50"/>
     </row>
     <row r="31" spans="1:20" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="72" t="str">
+      <c r="A31" s="67" t="str">
         <f>CONCATENATE("participant"," ",J6)</f>
         <v>participant CIS</v>
       </c>
-      <c r="B31" s="73"/>
+      <c r="B31" s="68"/>
       <c r="C31" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="D31" s="70" t="s">
+      <c r="D31" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="E31" s="74"/>
-      <c r="F31" s="74"/>
-      <c r="G31" s="74"/>
-      <c r="H31" s="74"/>
-      <c r="I31" s="74"/>
-      <c r="J31" s="74"/>
-      <c r="K31" s="74"/>
-      <c r="L31" s="74"/>
-      <c r="M31" s="74"/>
-      <c r="N31" s="74"/>
-      <c r="O31" s="74"/>
-      <c r="P31" s="74"/>
+      <c r="E31" s="72"/>
+      <c r="F31" s="72"/>
+      <c r="G31" s="72"/>
+      <c r="H31" s="72"/>
+      <c r="I31" s="72"/>
+      <c r="J31" s="72"/>
+      <c r="K31" s="72"/>
+      <c r="L31" s="72"/>
+      <c r="M31" s="72"/>
+      <c r="N31" s="72"/>
+      <c r="O31" s="72"/>
+      <c r="P31" s="72"/>
     </row>
     <row r="32" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="75" t="s">
+      <c r="A32" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="75"/>
-      <c r="C32" s="86">
+      <c r="B32" s="61"/>
+      <c r="C32" s="60">
         <v>51406</v>
       </c>
-      <c r="D32" s="76" t="s">
+      <c r="D32" s="73" t="s">
         <v>59</v>
       </c>
-      <c r="E32" s="77"/>
-      <c r="F32" s="77"/>
-      <c r="G32" s="77"/>
-      <c r="H32" s="77"/>
-      <c r="I32" s="77"/>
-      <c r="J32" s="77"/>
-      <c r="K32" s="77"/>
-      <c r="L32" s="77"/>
-      <c r="M32" s="77"/>
-      <c r="N32" s="77"/>
-      <c r="O32" s="77"/>
-      <c r="P32" s="77"/>
+      <c r="E32" s="66"/>
+      <c r="F32" s="66"/>
+      <c r="G32" s="66"/>
+      <c r="H32" s="66"/>
+      <c r="I32" s="66"/>
+      <c r="J32" s="66"/>
+      <c r="K32" s="66"/>
+      <c r="L32" s="66"/>
+      <c r="M32" s="66"/>
+      <c r="N32" s="66"/>
+      <c r="O32" s="66"/>
+      <c r="P32" s="66"/>
       <c r="S32" s="31"/>
     </row>
     <row r="33" spans="1:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="75" t="s">
+      <c r="A33" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="75"/>
+      <c r="B33" s="61"/>
       <c r="C33" s="35">
         <v>60000</v>
       </c>
-      <c r="D33" s="77" t="s">
+      <c r="D33" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="E33" s="77"/>
-      <c r="F33" s="77"/>
-      <c r="G33" s="77"/>
-      <c r="H33" s="77"/>
-      <c r="I33" s="77"/>
-      <c r="J33" s="77"/>
-      <c r="K33" s="77"/>
-      <c r="L33" s="77"/>
-      <c r="M33" s="77"/>
-      <c r="N33" s="77"/>
-      <c r="O33" s="77"/>
-      <c r="P33" s="77"/>
+      <c r="E33" s="66"/>
+      <c r="F33" s="66"/>
+      <c r="G33" s="66"/>
+      <c r="H33" s="66"/>
+      <c r="I33" s="66"/>
+      <c r="J33" s="66"/>
+      <c r="K33" s="66"/>
+      <c r="L33" s="66"/>
+      <c r="M33" s="66"/>
+      <c r="N33" s="66"/>
+      <c r="O33" s="66"/>
+      <c r="P33" s="66"/>
       <c r="S33" s="31"/>
     </row>
     <row r="34" spans="1:19" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="75" t="s">
+      <c r="A34" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="75"/>
+      <c r="B34" s="61"/>
       <c r="C34" s="35">
         <v>19000</v>
       </c>
-      <c r="D34" s="77"/>
-      <c r="E34" s="77"/>
-      <c r="F34" s="77"/>
-      <c r="G34" s="77"/>
-      <c r="H34" s="77"/>
-      <c r="I34" s="77"/>
-      <c r="J34" s="77"/>
-      <c r="K34" s="77"/>
-      <c r="L34" s="77"/>
-      <c r="M34" s="77"/>
-      <c r="N34" s="77"/>
-      <c r="O34" s="77"/>
-      <c r="P34" s="77"/>
+      <c r="D34" s="66"/>
+      <c r="E34" s="66"/>
+      <c r="F34" s="66"/>
+      <c r="G34" s="66"/>
+      <c r="H34" s="66"/>
+      <c r="I34" s="66"/>
+      <c r="J34" s="66"/>
+      <c r="K34" s="66"/>
+      <c r="L34" s="66"/>
+      <c r="M34" s="66"/>
+      <c r="N34" s="66"/>
+      <c r="O34" s="66"/>
+      <c r="P34" s="66"/>
       <c r="S34" s="31"/>
     </row>
     <row r="35" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
@@ -3808,97 +3819,99 @@
       <c r="P36" s="38"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A37" s="72" t="str">
+      <c r="A37" s="67" t="str">
         <f>CONCATENATE("participant"," ",C9)</f>
         <v xml:space="preserve">participant </v>
       </c>
-      <c r="B37" s="73"/>
+      <c r="B37" s="68"/>
       <c r="C37" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="D37" s="82" t="s">
+      <c r="D37" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="E37" s="83"/>
-      <c r="F37" s="83"/>
-      <c r="G37" s="83"/>
-      <c r="H37" s="83"/>
-      <c r="I37" s="83"/>
-      <c r="J37" s="83"/>
-      <c r="K37" s="83"/>
-      <c r="L37" s="83"/>
-      <c r="M37" s="83"/>
-      <c r="N37" s="83"/>
-      <c r="O37" s="83"/>
-      <c r="P37" s="83"/>
+      <c r="E37" s="70"/>
+      <c r="F37" s="70"/>
+      <c r="G37" s="70"/>
+      <c r="H37" s="70"/>
+      <c r="I37" s="70"/>
+      <c r="J37" s="70"/>
+      <c r="K37" s="70"/>
+      <c r="L37" s="70"/>
+      <c r="M37" s="70"/>
+      <c r="N37" s="70"/>
+      <c r="O37" s="70"/>
+      <c r="P37" s="70"/>
     </row>
     <row r="38" spans="1:19" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="75" t="s">
+      <c r="A38" s="61" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="75"/>
-      <c r="C38" s="35"/>
-      <c r="D38" s="81" t="s">
+      <c r="B38" s="61"/>
+      <c r="C38" s="35">
+        <v>20000</v>
+      </c>
+      <c r="D38" s="65" t="s">
         <v>61</v>
       </c>
-      <c r="E38" s="77"/>
-      <c r="F38" s="77"/>
-      <c r="G38" s="77"/>
-      <c r="H38" s="77"/>
-      <c r="I38" s="77"/>
-      <c r="J38" s="77"/>
-      <c r="K38" s="77"/>
-      <c r="L38" s="77"/>
-      <c r="M38" s="77"/>
-      <c r="N38" s="77"/>
-      <c r="O38" s="77"/>
-      <c r="P38" s="77"/>
+      <c r="E38" s="66"/>
+      <c r="F38" s="66"/>
+      <c r="G38" s="66"/>
+      <c r="H38" s="66"/>
+      <c r="I38" s="66"/>
+      <c r="J38" s="66"/>
+      <c r="K38" s="66"/>
+      <c r="L38" s="66"/>
+      <c r="M38" s="66"/>
+      <c r="N38" s="66"/>
+      <c r="O38" s="66"/>
+      <c r="P38" s="66"/>
       <c r="S38" s="31"/>
     </row>
     <row r="39" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="75" t="s">
+      <c r="A39" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="75"/>
+      <c r="B39" s="61"/>
       <c r="C39" s="35"/>
-      <c r="D39" s="78" t="s">
+      <c r="D39" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="E39" s="79"/>
-      <c r="F39" s="79"/>
-      <c r="G39" s="79"/>
-      <c r="H39" s="79"/>
-      <c r="I39" s="79"/>
-      <c r="J39" s="79"/>
-      <c r="K39" s="79"/>
-      <c r="L39" s="79"/>
-      <c r="M39" s="79"/>
-      <c r="N39" s="79"/>
-      <c r="O39" s="79"/>
-      <c r="P39" s="80"/>
+      <c r="E39" s="63"/>
+      <c r="F39" s="63"/>
+      <c r="G39" s="63"/>
+      <c r="H39" s="63"/>
+      <c r="I39" s="63"/>
+      <c r="J39" s="63"/>
+      <c r="K39" s="63"/>
+      <c r="L39" s="63"/>
+      <c r="M39" s="63"/>
+      <c r="N39" s="63"/>
+      <c r="O39" s="63"/>
+      <c r="P39" s="64"/>
       <c r="S39" s="31"/>
     </row>
     <row r="40" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="75" t="s">
+      <c r="A40" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="75"/>
+      <c r="B40" s="61"/>
       <c r="C40" s="35"/>
-      <c r="D40" s="81" t="s">
+      <c r="D40" s="65" t="s">
         <v>41</v>
       </c>
-      <c r="E40" s="77"/>
-      <c r="F40" s="77"/>
-      <c r="G40" s="77"/>
-      <c r="H40" s="77"/>
-      <c r="I40" s="77"/>
-      <c r="J40" s="77"/>
-      <c r="K40" s="77"/>
-      <c r="L40" s="77"/>
-      <c r="M40" s="77"/>
-      <c r="N40" s="77"/>
-      <c r="O40" s="77"/>
-      <c r="P40" s="77"/>
+      <c r="E40" s="66"/>
+      <c r="F40" s="66"/>
+      <c r="G40" s="66"/>
+      <c r="H40" s="66"/>
+      <c r="I40" s="66"/>
+      <c r="J40" s="66"/>
+      <c r="K40" s="66"/>
+      <c r="L40" s="66"/>
+      <c r="M40" s="66"/>
+      <c r="N40" s="66"/>
+      <c r="O40" s="66"/>
+      <c r="P40" s="66"/>
       <c r="S40" s="31"/>
     </row>
   </sheetData>
@@ -3906,34 +3919,6 @@
     <protectedRange sqref="C32:P40 D14:H23 P14:P23 O6 J14:N23 R14:S23" name="Range1"/>
   </protectedRanges>
   <mergeCells count="41">
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:P39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:P40"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D34:P34"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:P37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:P38"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:P31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:P32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:P33"/>
-    <mergeCell ref="A28:P28"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:C24"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="E3:I3"/>
     <mergeCell ref="E4:I4"/>
@@ -3947,6 +3932,34 @@
     <mergeCell ref="A10:R10"/>
     <mergeCell ref="D12:I12"/>
     <mergeCell ref="J12:R12"/>
+    <mergeCell ref="A28:P28"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:P31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:P32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:P33"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:P39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:P40"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D34:P34"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:P37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:P38"/>
   </mergeCells>
   <conditionalFormatting sqref="O4">
     <cfRule type="expression" dxfId="0" priority="1">
@@ -3967,11 +3980,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="B1:T65"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P42" sqref="P42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4003,7 +4015,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="2:16" ht="160.80000000000001" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:16" ht="161.4" x14ac:dyDescent="0.3">
       <c r="B4" s="41" t="s">
         <v>52</v>
       </c>
@@ -4050,7 +4062,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="2:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="39" t="s">
         <v>64</v>
       </c>
@@ -4092,7 +4104,7 @@
         <v>5720</v>
       </c>
     </row>
-    <row r="6" spans="2:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" s="52" t="s">
         <v>64</v>
       </c>
@@ -4176,7 +4188,7 @@
         <v>5720</v>
       </c>
     </row>
-    <row r="8" spans="2:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8" s="52" t="s">
         <v>64</v>
       </c>
@@ -4218,7 +4230,7 @@
         <v>5720</v>
       </c>
     </row>
-    <row r="9" spans="2:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9" s="52" t="s">
         <v>64</v>
       </c>
@@ -4260,7 +4272,7 @@
         <v>5720</v>
       </c>
     </row>
-    <row r="10" spans="2:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" s="39" t="s">
         <v>71</v>
       </c>
@@ -4308,7 +4320,7 @@
         <v>26175</v>
       </c>
     </row>
-    <row r="11" spans="2:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B11" s="52" t="s">
         <v>71</v>
       </c>
@@ -4356,7 +4368,7 @@
         <v>20940</v>
       </c>
     </row>
-    <row r="12" spans="2:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B12" s="52" t="s">
         <v>71</v>
       </c>
@@ -4400,7 +4412,7 @@
         <v>13960</v>
       </c>
     </row>
-    <row r="13" spans="2:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B13" s="39" t="s">
         <v>72</v>
       </c>
@@ -4450,7 +4462,7 @@
         <v>25466</v>
       </c>
     </row>
-    <row r="14" spans="2:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B14" s="52" t="s">
         <v>72</v>
       </c>
@@ -4544,7 +4556,7 @@
         <v>10486</v>
       </c>
     </row>
-    <row r="16" spans="2:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B16" s="52" t="s">
         <v>72</v>
       </c>
@@ -4588,7 +4600,7 @@
         <v>8074</v>
       </c>
     </row>
-    <row r="17" spans="2:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B17" s="52" t="s">
         <v>72</v>
       </c>
@@ -4632,7 +4644,7 @@
         <v>9576</v>
       </c>
     </row>
-    <row r="18" spans="2:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B18" s="39" t="s">
         <v>73</v>
       </c>
@@ -4722,7 +4734,7 @@
         <v>11440</v>
       </c>
     </row>
-    <row r="20" spans="2:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B20" s="52" t="s">
         <v>73</v>
       </c>
@@ -4768,7 +4780,7 @@
         <v>15400</v>
       </c>
     </row>
-    <row r="21" spans="2:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B21" s="39" t="s">
         <v>109</v>
       </c>
@@ -4816,7 +4828,7 @@
         <v>15470</v>
       </c>
     </row>
-    <row r="22" spans="2:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B22" s="52" t="s">
         <v>109</v>
       </c>
@@ -4862,7 +4874,7 @@
         <v>9520</v>
       </c>
     </row>
-    <row r="23" spans="2:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B23" s="52" t="s">
         <v>109</v>
       </c>
@@ -4950,7 +4962,7 @@
         <v>9120</v>
       </c>
     </row>
-    <row r="25" spans="2:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B25" s="52" t="s">
         <v>109</v>
       </c>
@@ -4998,7 +5010,7 @@
         <v>13680</v>
       </c>
     </row>
-    <row r="26" spans="2:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B26" s="52" t="s">
         <v>109</v>
       </c>
@@ -5044,7 +5056,7 @@
         <v>12160</v>
       </c>
     </row>
-    <row r="27" spans="2:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B27" s="39" t="s">
         <v>64</v>
       </c>
@@ -5092,7 +5104,7 @@
         <v>17658</v>
       </c>
     </row>
-    <row r="28" spans="2:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B28" s="52" t="s">
         <v>64</v>
       </c>
@@ -5136,7 +5148,7 @@
         <v>11772</v>
       </c>
     </row>
-    <row r="29" spans="2:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B29" s="52" t="s">
         <v>64</v>
       </c>
@@ -5182,7 +5194,7 @@
         <v>11772</v>
       </c>
     </row>
-    <row r="30" spans="2:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B30" s="39" t="s">
         <v>110</v>
       </c>
@@ -5230,7 +5242,7 @@
         <v>30184</v>
       </c>
     </row>
-    <row r="31" spans="2:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B31" s="52" t="s">
         <v>110</v>
       </c>
@@ -5276,7 +5288,7 @@
         <v>14462</v>
       </c>
     </row>
-    <row r="32" spans="2:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B32" s="52" t="s">
         <v>110</v>
       </c>
@@ -5322,7 +5334,7 @@
         <v>19404</v>
       </c>
     </row>
-    <row r="33" spans="2:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B33" s="52" t="s">
         <v>110</v>
       </c>
@@ -5368,7 +5380,7 @@
         <v>19404</v>
       </c>
     </row>
-    <row r="34" spans="2:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B34" s="39" t="s">
         <v>111</v>
       </c>
@@ -5412,7 +5424,7 @@
         <v>12810</v>
       </c>
     </row>
-    <row r="35" spans="2:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B35" s="39" t="s">
         <v>111</v>
       </c>
@@ -5500,7 +5512,7 @@
         <v>14640</v>
       </c>
     </row>
-    <row r="37" spans="2:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B37" s="52" t="s">
         <v>111</v>
       </c>
@@ -5544,7 +5556,7 @@
         <v>16470</v>
       </c>
     </row>
-    <row r="38" spans="2:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B38" s="52" t="s">
         <v>111</v>
       </c>
@@ -5592,10 +5604,10 @@
         <v>24990</v>
       </c>
     </row>
-    <row r="39" spans="2:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:16" x14ac:dyDescent="0.3">
       <c r="P39" s="57"/>
     </row>
-    <row r="40" spans="2:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:16" x14ac:dyDescent="0.3">
       <c r="P40" s="57"/>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.3">
@@ -5714,13 +5726,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B4:P40" xr:uid="{47F2FC3E-A1F8-40C9-A910-B49FA41A830B}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="CIS"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="B4:P40" xr:uid="{47F2FC3E-A1F8-40C9-A910-B49FA41A830B}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:P16">
     <sortCondition ref="B5"/>
   </sortState>
@@ -5752,7 +5758,7 @@
   <dimension ref="B1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5805,7 +5811,7 @@
       <c r="B5" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="C5" s="59" t="s">
+      <c r="C5" s="58" t="s">
         <v>92</v>
       </c>
       <c r="D5" s="52" t="s">
@@ -5832,7 +5838,7 @@
       <c r="B6" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="58" t="s">
+      <c r="C6" s="86" t="s">
         <v>94</v>
       </c>
       <c r="D6" s="39" t="s">
@@ -5967,7 +5973,7 @@
       <c r="B11" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="C11" s="58" t="s">
+      <c r="C11" s="86" t="s">
         <v>94</v>
       </c>
       <c r="D11" s="39" t="s">
@@ -5994,7 +6000,7 @@
       <c r="B12" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="59" t="s">
+      <c r="C12" s="58" t="s">
         <v>92</v>
       </c>
       <c r="D12" s="39" t="s">
@@ -6129,7 +6135,7 @@
       <c r="B17" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="C17" s="59" t="s">
+      <c r="C17" s="58" t="s">
         <v>92</v>
       </c>
       <c r="D17" s="39" t="s">
@@ -6425,7 +6431,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8638632-8991-497A-A4ED-8B1346B51BB4}">
   <dimension ref="B1:I35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>

</xml_diff>